<commit_message>
Agregando la función "clasifica_bases()"
Y corrigiendo errores menores
</commit_message>
<xml_diff>
--- a/integracion_snmb/dependencias/fusionar_bases/relacion_esquemas_clientes_fusionadores.xlsx
+++ b/integracion_snmb/dependencias/fusionar_bases/relacion_esquemas_clientes_fusionadores.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fpardo/Desktop/conabio/nuevo_proceso_integracion_snmb/dependencias/fusionar_bases/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fpardo/Desktop/conabio/integracion_snmb_reestructurado/integracion_snmb/dependencias/fusionar_bases/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -444,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>